<commit_message>
- execute workflow - needleman
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/PHD/DS_Bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/PHD/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1199D951-646B-AB4D-8A27-A187167C7811}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779CFFC9-AB0B-E84B-AB0B-5B2EFD984D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="2240" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="26">
   <si>
     <t>ds</t>
   </si>
@@ -77,6 +78,42 @@
   </si>
   <si>
     <t>lowVarRemove</t>
+  </si>
+  <si>
+    <t>missingValues</t>
+  </si>
+  <si>
+    <t>zeroVariance</t>
+  </si>
+  <si>
+    <t>missingValues, zeroVariance</t>
+  </si>
+  <si>
+    <t>outliers</t>
+  </si>
+  <si>
+    <t>outliersRemoval</t>
+  </si>
+  <si>
+    <t>pca2</t>
+  </si>
+  <si>
+    <t>pearson</t>
+  </si>
+  <si>
+    <t>clustermap</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>oneHotEncode</t>
+  </si>
+  <si>
+    <t>missingValues, categorical</t>
+  </si>
+  <si>
+    <t>missingValuesRemove</t>
   </si>
 </sst>
 </file>
@@ -1332,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1347,92 +1384,101 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1440,10 +1486,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1457,19 +1503,124 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35202B10-EF9C-E146-B10F-6C6531951459}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- intermediate representation - adjust functions
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/PHD/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779CFFC9-AB0B-E84B-AB0B-5B2EFD984D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1F1229-A48D-F245-8A15-A38C2F9173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="2240" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
+    <workbookView xWindow="3480" yWindow="1920" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="35">
   <si>
     <t>ds</t>
   </si>
@@ -92,9 +92,6 @@
     <t>outliers</t>
   </si>
   <si>
-    <t>outliersRemoval</t>
-  </si>
-  <si>
     <t>pca2</t>
   </si>
   <si>
@@ -114,6 +111,36 @@
   </si>
   <si>
     <t>missingValuesRemove</t>
+  </si>
+  <si>
+    <t>agglomerativeClustering</t>
+  </si>
+  <si>
+    <t>missingValues, hasLabel</t>
+  </si>
+  <si>
+    <t>zeroVariance, hasLabel</t>
+  </si>
+  <si>
+    <t>missingValues, zeroVariance, hasLabel</t>
+  </si>
+  <si>
+    <t>hasLabel</t>
+  </si>
+  <si>
+    <t>outliers, hasLabel</t>
+  </si>
+  <si>
+    <t>categorical, hasLabel</t>
+  </si>
+  <si>
+    <t>missingValues, categorical, hasLabel</t>
+  </si>
+  <si>
+    <t>labelRemove</t>
+  </si>
+  <si>
+    <t>outliersRemove</t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1393,7 +1420,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -1407,27 +1434,27 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1438,174 +1465,715 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>19</v>
       </c>
-      <c r="F14" t="s">
-        <v>5</v>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fix ir implementations
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/PHD/DSBot/DSBot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1F1229-A48D-F245-8A15-A38C2F9173C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09962862-ACCA-6845-96D2-A479AEB18C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="1920" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
+    <workbookView xWindow="5020" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="35">
   <si>
     <t>ds</t>
   </si>
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="F21" sqref="F21:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1753,6 +1753,9 @@
       <c r="E21" t="s">
         <v>18</v>
       </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1770,6 +1773,9 @@
       <c r="E22" t="s">
         <v>18</v>
       </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1961,7 +1967,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1979,7 +1985,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1991,7 +1997,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2011,7 +2017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -2048,7 +2054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -2079,7 +2085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -2099,7 +2105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -2119,7 +2125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -2155,8 +2161,11 @@
       <c r="F43" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -2174,6 +2183,9 @@
       </c>
       <c r="F44" t="s">
         <v>18</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fix pca2/pca3 - add to table
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09962862-ACCA-6845-96D2-A479AEB18C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EA54E8-263D-3344-8F99-AF5C77DB8DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="38">
   <si>
     <t>ds</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>outliersRemove</t>
+  </si>
+  <si>
+    <t>randomForest</t>
+  </si>
+  <si>
+    <t>missingValues, hasLabel, categorical</t>
+  </si>
+  <si>
+    <t>missingValues, hasLabel, zeroVariance</t>
   </si>
 </sst>
 </file>
@@ -1396,17 +1405,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2186,6 +2197,201 @@
       </c>
       <c r="G44" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- add laplace - modify kb - add mds
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EA54E8-263D-3344-8F99-AF5C77DB8DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B95B290-AEC1-BD42-9CBC-F87D9BE517CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -511,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4570536A-8F77-7445-8EA3-9DF409713A55}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="109" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -1407,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1625,17 +1626,14 @@
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1646,7 +1644,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
@@ -1660,12 +1658,15 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1674,7 +1675,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -1687,14 +1688,14 @@
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
+      <c r="B17" t="s">
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
- modified clustering - adding laplace to kb - fixing laplace
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B95B290-AEC1-BD42-9CBC-F87D9BE517CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF0BE3-8BBE-534B-A4C5-3B268AC86399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
+    <workbookView xWindow="4040" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="51">
   <si>
     <t>ds</t>
   </si>
@@ -151,6 +150,45 @@
   </si>
   <si>
     <t>missingValues, hasLabel, zeroVariance</t>
+  </si>
+  <si>
+    <t>laplace</t>
+  </si>
+  <si>
+    <t>missingValues, moreFeatures</t>
+  </si>
+  <si>
+    <t>zeroVariance, moreFeatures</t>
+  </si>
+  <si>
+    <t>outliers, moreFeatures</t>
+  </si>
+  <si>
+    <t>moreFeatures</t>
+  </si>
+  <si>
+    <t>categorical, moreFeatures</t>
+  </si>
+  <si>
+    <t>missingValues, categorical, moreFeatures</t>
+  </si>
+  <si>
+    <t>missingValues, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>missingValues, zeroVariance, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>outliers, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>categorical, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>missingValues, categorical, hasLabel, moreFeatures</t>
   </si>
 </sst>
 </file>
@@ -1406,15 +1444,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="64.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
@@ -2259,7 +2297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -2276,7 +2314,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -2293,7 +2331,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -2310,7 +2348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2327,7 +2365,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -2344,7 +2382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -2361,7 +2399,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -2378,7 +2416,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -2393,6 +2431,606 @@
       </c>
       <c r="E56" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>39</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" t="s">
+        <v>18</v>
+      </c>
+      <c r="H73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" t="s">
+        <v>18</v>
+      </c>
+      <c r="H74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>47</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" t="s">
+        <v>38</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" t="s">
+        <v>18</v>
+      </c>
+      <c r="G77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" t="s">
+        <v>38</v>
+      </c>
+      <c r="E78" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" t="s">
+        <v>18</v>
+      </c>
+      <c r="G78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C80" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80" t="s">
+        <v>25</v>
+      </c>
+      <c r="E80" t="s">
+        <v>18</v>
+      </c>
+      <c r="F80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D81" t="s">
+        <v>38</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
+      </c>
+      <c r="F81" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>49</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D82" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" t="s">
+        <v>25</v>
+      </c>
+      <c r="F82" t="s">
+        <v>18</v>
+      </c>
+      <c r="G82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" t="s">
+        <v>18</v>
+      </c>
+      <c r="H83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" t="s">
+        <v>18</v>
+      </c>
+      <c r="H84" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- add rows to kb
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF0BE3-8BBE-534B-A4C5-3B268AC86399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297796E5-6A8F-5A4A-A991-7AA05040004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="53">
   <si>
     <t>ds</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>missingValues, categorical, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>missingValues, zeroVariance, moreFeatures</t>
+  </si>
+  <si>
+    <t>zeroVariance, hasLabel, moreFeatures</t>
   </si>
 </sst>
 </file>
@@ -1444,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="E147" sqref="E147:G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1783,9 +1789,6 @@
       <c r="D20" t="s">
         <v>20</v>
       </c>
-      <c r="F20" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1829,22 +1832,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1858,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
         <v>18</v>
@@ -1871,54 +1871,51 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
-        <v>1</v>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1928,16 +1925,22 @@
       <c r="B28" t="s">
         <v>11</v>
       </c>
-      <c r="C28" t="s">
-        <v>19</v>
+      <c r="C28" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -1946,21 +1949,15 @@
         <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1969,181 +1966,185 @@
         <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E35" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" t="s">
-        <v>5</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E36" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" t="s">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E37" t="s">
         <v>5</v>
       </c>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" t="s">
-        <v>5</v>
-      </c>
+      <c r="C38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
@@ -2157,13 +2158,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D41" t="s">
         <v>25</v>
@@ -2177,146 +2178,143 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>33</v>
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E43" t="s">
-        <v>6</v>
-      </c>
-      <c r="F43" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>35</v>
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
       <c r="E48" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E49" t="s">
-        <v>35</v>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>24</v>
@@ -2324,33 +2322,45 @@
       <c r="C50" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>22</v>
       </c>
       <c r="E50" t="s">
-        <v>35</v>
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>33</v>
+      <c r="C51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" t="s">
+        <v>22</v>
       </c>
       <c r="E51" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>24</v>
@@ -2358,16 +2368,19 @@
       <c r="C52" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>33</v>
+      <c r="D52" t="s">
+        <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>24</v>
@@ -2375,16 +2388,13 @@
       <c r="C53" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="D53" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>24</v>
@@ -2392,16 +2402,13 @@
       <c r="C54" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="D54" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>24</v>
@@ -2409,10 +2416,7 @@
       <c r="C55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D55" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2435,202 +2439,186 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
+        <v>36</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D58" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E58" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>40</v>
-      </c>
-      <c r="B59" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E60" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E61" t="s">
-        <v>5</v>
-      </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>41</v>
-      </c>
-      <c r="B63" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63" t="s">
-        <v>38</v>
-      </c>
-      <c r="D63" t="s">
-        <v>6</v>
+        <v>36</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E63" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
         <v>38</v>
       </c>
-      <c r="D64" t="s">
-        <v>25</v>
-      </c>
-      <c r="E64" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
         <v>38</v>
       </c>
-      <c r="C65" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" t="s">
-        <v>25</v>
-      </c>
       <c r="D66" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>43</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
       </c>
       <c r="C67" t="s">
         <v>38</v>
@@ -2645,12 +2633,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>43</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
       </c>
       <c r="C68" t="s">
         <v>38</v>
@@ -2665,156 +2653,124 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>44</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>41</v>
+      </c>
+      <c r="B71" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D69" t="s">
-        <v>38</v>
-      </c>
-      <c r="E69" t="s">
-        <v>6</v>
-      </c>
-      <c r="F69" t="s">
-        <v>18</v>
-      </c>
-      <c r="G69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" t="s">
-        <v>22</v>
-      </c>
-      <c r="D70" t="s">
-        <v>38</v>
-      </c>
-      <c r="E70" t="s">
-        <v>25</v>
-      </c>
-      <c r="F70" t="s">
-        <v>18</v>
-      </c>
-      <c r="G70" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>45</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
-        <v>38</v>
-      </c>
-      <c r="E71" t="s">
-        <v>6</v>
-      </c>
-      <c r="F71" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>45</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" t="s">
-        <v>38</v>
-      </c>
-      <c r="E72" t="s">
-        <v>25</v>
-      </c>
-      <c r="F72" t="s">
-        <v>18</v>
-      </c>
-      <c r="G72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>46</v>
-      </c>
-      <c r="B73" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D73" t="s">
-        <v>1</v>
-      </c>
-      <c r="E73" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" t="s">
-        <v>6</v>
-      </c>
-      <c r="G73" t="s">
-        <v>18</v>
-      </c>
-      <c r="H73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>46</v>
-      </c>
-      <c r="B74" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D74" t="s">
-        <v>1</v>
-      </c>
-      <c r="E74" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" t="s">
-        <v>25</v>
-      </c>
-      <c r="G74" t="s">
-        <v>18</v>
-      </c>
-      <c r="H74" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>47</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C75" t="s">
         <v>38</v>
@@ -2829,12 +2785,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C76" t="s">
         <v>38</v>
@@ -2849,15 +2805,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>48</v>
-      </c>
-      <c r="B77" t="s">
-        <v>34</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" t="s">
+        <v>22</v>
       </c>
       <c r="D77" t="s">
         <v>38</v>
@@ -2872,15 +2828,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>48</v>
-      </c>
-      <c r="B78" t="s">
-        <v>34</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" t="s">
+        <v>22</v>
       </c>
       <c r="D78" t="s">
         <v>38</v>
@@ -2895,142 +2851,1340 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
         <v>38</v>
       </c>
-      <c r="D79" t="s">
-        <v>6</v>
-      </c>
       <c r="E79" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
         <v>38</v>
       </c>
-      <c r="D80" t="s">
-        <v>25</v>
-      </c>
       <c r="E80" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F80" t="s">
+        <v>18</v>
+      </c>
+      <c r="G80" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>49</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
         <v>38</v>
       </c>
-      <c r="E81" t="s">
-        <v>6</v>
-      </c>
       <c r="F81" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G81" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>49</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D82" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
         <v>38</v>
       </c>
-      <c r="E82" t="s">
-        <v>25</v>
-      </c>
       <c r="F82" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G82" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>33</v>
+        <v>33</v>
+      </c>
+      <c r="C83" t="s">
+        <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E83" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F83" t="s">
-        <v>6</v>
-      </c>
-      <c r="G83" t="s">
-        <v>18</v>
-      </c>
-      <c r="H83" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" t="s">
+        <v>25</v>
+      </c>
+      <c r="E84" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>48</v>
+      </c>
+      <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" t="s">
+        <v>38</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>48</v>
+      </c>
+      <c r="B86" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" t="s">
+        <v>38</v>
+      </c>
+      <c r="E86" t="s">
+        <v>25</v>
+      </c>
+      <c r="F86" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>48</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" t="s">
+        <v>38</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>48</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" t="s">
+        <v>38</v>
+      </c>
+      <c r="D88" t="s">
+        <v>25</v>
+      </c>
+      <c r="E88" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>49</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" t="s">
+        <v>38</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" t="s">
+        <v>18</v>
+      </c>
+      <c r="G89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" t="s">
+        <v>38</v>
+      </c>
+      <c r="E90" t="s">
+        <v>25</v>
+      </c>
+      <c r="F90" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>50</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="C91" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" t="s">
         <v>22</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E91" t="s">
         <v>38</v>
       </c>
-      <c r="F84" t="s">
-        <v>25</v>
-      </c>
-      <c r="G84" t="s">
-        <v>18</v>
-      </c>
-      <c r="H84" t="s">
-        <v>5</v>
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>50</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" t="s">
+        <v>18</v>
+      </c>
+      <c r="H92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" t="s">
+        <v>25</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" t="s">
+        <v>5</v>
+      </c>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>39</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>25</v>
+      </c>
+      <c r="D98" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>40</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" t="s">
+        <v>18</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>40</v>
+      </c>
+      <c r="B100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" t="s">
+        <v>25</v>
+      </c>
+      <c r="D100" t="s">
+        <v>18</v>
+      </c>
+      <c r="E100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>41</v>
+      </c>
+      <c r="B101" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" t="s">
+        <v>18</v>
+      </c>
+      <c r="E101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" t="s">
+        <v>34</v>
+      </c>
+      <c r="C102" t="s">
+        <v>25</v>
+      </c>
+      <c r="D102" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>41</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>41</v>
+      </c>
+      <c r="B104" t="s">
+        <v>25</v>
+      </c>
+      <c r="C104" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>43</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>43</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C108" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" t="s">
+        <v>25</v>
+      </c>
+      <c r="E108" t="s">
+        <v>18</v>
+      </c>
+      <c r="F108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>45</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" t="s">
+        <v>18</v>
+      </c>
+      <c r="F109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>45</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E110" t="s">
+        <v>18</v>
+      </c>
+      <c r="F110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>46</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>6</v>
+      </c>
+      <c r="F111" t="s">
+        <v>18</v>
+      </c>
+      <c r="G111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>46</v>
+      </c>
+      <c r="B112" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>25</v>
+      </c>
+      <c r="F112" t="s">
+        <v>18</v>
+      </c>
+      <c r="G112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>47</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C113" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" t="s">
+        <v>18</v>
+      </c>
+      <c r="E113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>47</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C114" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" t="s">
+        <v>18</v>
+      </c>
+      <c r="E114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>48</v>
+      </c>
+      <c r="B115" t="s">
+        <v>34</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" t="s">
+        <v>18</v>
+      </c>
+      <c r="F115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>48</v>
+      </c>
+      <c r="B116" t="s">
+        <v>34</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D116" t="s">
+        <v>25</v>
+      </c>
+      <c r="E116" t="s">
+        <v>18</v>
+      </c>
+      <c r="F116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>48</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C117" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" t="s">
+        <v>18</v>
+      </c>
+      <c r="E117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>48</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C118" t="s">
+        <v>25</v>
+      </c>
+      <c r="D118" t="s">
+        <v>18</v>
+      </c>
+      <c r="E118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>49</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" t="s">
+        <v>18</v>
+      </c>
+      <c r="F119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>49</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D120" t="s">
+        <v>25</v>
+      </c>
+      <c r="E120" t="s">
+        <v>18</v>
+      </c>
+      <c r="F120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>50</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D121" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121" t="s">
+        <v>6</v>
+      </c>
+      <c r="F121" t="s">
+        <v>18</v>
+      </c>
+      <c r="G121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>50</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D122" t="s">
+        <v>22</v>
+      </c>
+      <c r="E122" t="s">
+        <v>25</v>
+      </c>
+      <c r="F122" t="s">
+        <v>18</v>
+      </c>
+      <c r="G122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>39</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D123" t="s">
+        <v>19</v>
+      </c>
+      <c r="E123" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>39</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>40</v>
+      </c>
+      <c r="B125" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D125" t="s">
+        <v>19</v>
+      </c>
+      <c r="E125" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>40</v>
+      </c>
+      <c r="B126" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" t="s">
+        <v>19</v>
+      </c>
+      <c r="D126" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>51</v>
+      </c>
+      <c r="B127" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E127" t="s">
+        <v>19</v>
+      </c>
+      <c r="F127" t="s">
+        <v>20</v>
+      </c>
+      <c r="G127" s="1"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>51</v>
+      </c>
+      <c r="B128" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128" t="s">
+        <v>19</v>
+      </c>
+      <c r="E128" t="s">
+        <v>20</v>
+      </c>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>41</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D129" t="s">
+        <v>19</v>
+      </c>
+      <c r="E129" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>41</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C130" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>43</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D131" t="s">
+        <v>19</v>
+      </c>
+      <c r="E131" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>43</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132" t="s">
+        <v>19</v>
+      </c>
+      <c r="D132" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>44</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C133" t="s">
+        <v>22</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E133" t="s">
+        <v>19</v>
+      </c>
+      <c r="F133" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>44</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C134" t="s">
+        <v>22</v>
+      </c>
+      <c r="D134" t="s">
+        <v>19</v>
+      </c>
+      <c r="E134" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>45</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E135" t="s">
+        <v>19</v>
+      </c>
+      <c r="F135" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>45</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1</v>
+      </c>
+      <c r="D136" t="s">
+        <v>19</v>
+      </c>
+      <c r="E136" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>52</v>
+      </c>
+      <c r="B137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E137" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>52</v>
+      </c>
+      <c r="B138" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138" t="s">
+        <v>19</v>
+      </c>
+      <c r="E138" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>46</v>
+      </c>
+      <c r="B139" t="s">
+        <v>11</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F139" t="s">
+        <v>19</v>
+      </c>
+      <c r="G139" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>46</v>
+      </c>
+      <c r="B140" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D140" t="s">
+        <v>1</v>
+      </c>
+      <c r="E140" t="s">
+        <v>19</v>
+      </c>
+      <c r="F140" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>47</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D141" t="s">
+        <v>19</v>
+      </c>
+      <c r="E141" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>47</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>48</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E143" t="s">
+        <v>19</v>
+      </c>
+      <c r="F143" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>48</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D144" t="s">
+        <v>19</v>
+      </c>
+      <c r="E144" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>49</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E145" t="s">
+        <v>19</v>
+      </c>
+      <c r="F145" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>50</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D147" t="s">
+        <v>22</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F147" t="s">
+        <v>19</v>
+      </c>
+      <c r="G147" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>50</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D148" t="s">
+        <v>22</v>
+      </c>
+      <c r="E148" t="s">
+        <v>19</v>
+      </c>
+      <c r="F148" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- add rows to kb - add implementations - add details to show to user
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297796E5-6A8F-5A4A-A991-7AA05040004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EF5CD1-A4C1-BE45-BBB6-5FD0B374BEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
+    <workbookView xWindow="4020" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
-    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
+    <sheet name="Foglio4" sheetId="4" r:id="rId3"/>
+    <sheet name="Foglio3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="56">
   <si>
     <t>ds</t>
   </si>
@@ -195,6 +196,15 @@
   </si>
   <si>
     <t>zeroVariance, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>distplot</t>
+  </si>
+  <si>
+    <t>barplot</t>
+  </si>
+  <si>
+    <t>boxplot</t>
   </si>
 </sst>
 </file>
@@ -1450,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147:G147"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A149" sqref="A149:XFD232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4187,12 +4197,4172 @@
         <v>20</v>
       </c>
     </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C151" s="1"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D152" s="1"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B156" s="1"/>
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C159" s="1"/>
+      <c r="E159" s="1"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D166" s="1"/>
+    </row>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+    </row>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B170" s="1"/>
+      <c r="D170" s="1"/>
+    </row>
+    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+    </row>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+    </row>
+    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C173" s="1"/>
+      <c r="E173" s="1"/>
+    </row>
+    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+    </row>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D180" s="1"/>
+    </row>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+    </row>
+    <row r="182" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B182" s="1"/>
+    </row>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+    </row>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B184" s="1"/>
+      <c r="D184" s="1"/>
+    </row>
+    <row r="185" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1"/>
+    </row>
+    <row r="186" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+    </row>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C187" s="1"/>
+      <c r="E187" s="1"/>
+    </row>
+    <row r="188" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C188" s="1"/>
+      <c r="D188" s="1"/>
+      <c r="E188" s="1"/>
+    </row>
+    <row r="189" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B189" s="1"/>
+      <c r="C189" s="1"/>
+    </row>
+    <row r="190" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C190" s="1"/>
+      <c r="D190" s="1"/>
+    </row>
+    <row r="191" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B191" s="1"/>
+      <c r="C191" s="1"/>
+    </row>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+    </row>
+    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C193" s="1"/>
+    </row>
+    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D194" s="1"/>
+    </row>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C195" s="1"/>
+      <c r="D195" s="1"/>
+    </row>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B196" s="1"/>
+    </row>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+    </row>
+    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B198" s="1"/>
+      <c r="D198" s="1"/>
+    </row>
+    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B199" s="1"/>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1"/>
+    </row>
+    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C200" s="1"/>
+      <c r="D200" s="1"/>
+    </row>
+    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C201" s="1"/>
+      <c r="E201" s="1"/>
+    </row>
+    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C202" s="1"/>
+      <c r="D202" s="1"/>
+      <c r="E202" s="1"/>
+    </row>
+    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+    </row>
+    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+    </row>
+    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+    </row>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B206" s="1"/>
+      <c r="C206" s="1"/>
+    </row>
+    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C207" s="1"/>
+    </row>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D208" s="1"/>
+    </row>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C209" s="1"/>
+      <c r="D209" s="1"/>
+    </row>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B210" s="1"/>
+    </row>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B211" s="1"/>
+      <c r="C211" s="1"/>
+    </row>
+    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B212" s="1"/>
+      <c r="D212" s="1"/>
+    </row>
+    <row r="213" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B213" s="1"/>
+      <c r="C213" s="1"/>
+      <c r="D213" s="1"/>
+    </row>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C214" s="1"/>
+      <c r="D214" s="1"/>
+    </row>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C215" s="1"/>
+      <c r="E215" s="1"/>
+    </row>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C216" s="1"/>
+      <c r="D216" s="1"/>
+      <c r="E216" s="1"/>
+    </row>
+    <row r="217" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
+    </row>
+    <row r="218" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C218" s="1"/>
+      <c r="D218" s="1"/>
+    </row>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+    </row>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
+    </row>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C221" s="1"/>
+    </row>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D222" s="1"/>
+    </row>
+    <row r="223" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C223" s="1"/>
+      <c r="D223" s="1"/>
+    </row>
+    <row r="224" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B224" s="1"/>
+    </row>
+    <row r="225" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B225" s="1"/>
+      <c r="C225" s="1"/>
+    </row>
+    <row r="226" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B226" s="1"/>
+      <c r="D226" s="1"/>
+    </row>
+    <row r="227" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B227" s="1"/>
+      <c r="C227" s="1"/>
+      <c r="D227" s="1"/>
+    </row>
+    <row r="228" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C228" s="1"/>
+      <c r="D228" s="1"/>
+    </row>
+    <row r="229" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C229" s="1"/>
+      <c r="E229" s="1"/>
+    </row>
+    <row r="230" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C230" s="1"/>
+      <c r="D230" s="1"/>
+      <c r="E230" s="1"/>
+    </row>
+    <row r="231" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B231" s="1"/>
+      <c r="C231" s="1"/>
+    </row>
+    <row r="232" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C232" s="1"/>
+      <c r="D232" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D2990A-F429-0248-9892-0EF6030E3150}">
+  <dimension ref="A1:H232"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="64.5" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>40</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>41</v>
+      </c>
+      <c r="B71" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C75" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>43</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>44</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77" t="s">
+        <v>38</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" t="s">
+        <v>18</v>
+      </c>
+      <c r="G77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>44</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" t="s">
+        <v>38</v>
+      </c>
+      <c r="E78" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" t="s">
+        <v>18</v>
+      </c>
+      <c r="G78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>45</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>38</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" t="s">
+        <v>18</v>
+      </c>
+      <c r="G79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>38</v>
+      </c>
+      <c r="E80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F80" t="s">
+        <v>18</v>
+      </c>
+      <c r="G80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>46</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>47</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" t="s">
+        <v>18</v>
+      </c>
+      <c r="F83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" t="s">
+        <v>25</v>
+      </c>
+      <c r="E84" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>48</v>
+      </c>
+      <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" t="s">
+        <v>38</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>48</v>
+      </c>
+      <c r="B86" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" t="s">
+        <v>38</v>
+      </c>
+      <c r="E86" t="s">
+        <v>25</v>
+      </c>
+      <c r="F86" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>48</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" t="s">
+        <v>38</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>48</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" t="s">
+        <v>38</v>
+      </c>
+      <c r="D88" t="s">
+        <v>25</v>
+      </c>
+      <c r="E88" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>49</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" t="s">
+        <v>38</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" t="s">
+        <v>18</v>
+      </c>
+      <c r="G89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" t="s">
+        <v>38</v>
+      </c>
+      <c r="E90" t="s">
+        <v>25</v>
+      </c>
+      <c r="F90" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>50</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F91" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>50</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" t="s">
+        <v>18</v>
+      </c>
+      <c r="H92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" t="s">
+        <v>25</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" t="s">
+        <v>5</v>
+      </c>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>39</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>25</v>
+      </c>
+      <c r="D98" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>40</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" t="s">
+        <v>18</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>40</v>
+      </c>
+      <c r="B100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" t="s">
+        <v>25</v>
+      </c>
+      <c r="D100" t="s">
+        <v>18</v>
+      </c>
+      <c r="E100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>41</v>
+      </c>
+      <c r="B101" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" t="s">
+        <v>18</v>
+      </c>
+      <c r="E101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" t="s">
+        <v>34</v>
+      </c>
+      <c r="C102" t="s">
+        <v>25</v>
+      </c>
+      <c r="D102" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>41</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>41</v>
+      </c>
+      <c r="B104" t="s">
+        <v>25</v>
+      </c>
+      <c r="C104" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>43</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>43</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C108" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" t="s">
+        <v>25</v>
+      </c>
+      <c r="E108" t="s">
+        <v>18</v>
+      </c>
+      <c r="F108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>45</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" t="s">
+        <v>18</v>
+      </c>
+      <c r="F109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>45</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E110" t="s">
+        <v>18</v>
+      </c>
+      <c r="F110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>46</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>6</v>
+      </c>
+      <c r="F111" t="s">
+        <v>18</v>
+      </c>
+      <c r="G111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>46</v>
+      </c>
+      <c r="B112" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>25</v>
+      </c>
+      <c r="F112" t="s">
+        <v>18</v>
+      </c>
+      <c r="G112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>47</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C113" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" t="s">
+        <v>18</v>
+      </c>
+      <c r="E113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>47</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C114" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" t="s">
+        <v>18</v>
+      </c>
+      <c r="E114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>48</v>
+      </c>
+      <c r="B115" t="s">
+        <v>34</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" t="s">
+        <v>18</v>
+      </c>
+      <c r="F115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>48</v>
+      </c>
+      <c r="B116" t="s">
+        <v>34</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D116" t="s">
+        <v>25</v>
+      </c>
+      <c r="E116" t="s">
+        <v>18</v>
+      </c>
+      <c r="F116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>48</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C117" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" t="s">
+        <v>18</v>
+      </c>
+      <c r="E117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>48</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C118" t="s">
+        <v>25</v>
+      </c>
+      <c r="D118" t="s">
+        <v>18</v>
+      </c>
+      <c r="E118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>49</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" t="s">
+        <v>18</v>
+      </c>
+      <c r="F119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>49</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D120" t="s">
+        <v>25</v>
+      </c>
+      <c r="E120" t="s">
+        <v>18</v>
+      </c>
+      <c r="F120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>50</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D121" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121" t="s">
+        <v>6</v>
+      </c>
+      <c r="F121" t="s">
+        <v>18</v>
+      </c>
+      <c r="G121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>50</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D122" t="s">
+        <v>22</v>
+      </c>
+      <c r="E122" t="s">
+        <v>25</v>
+      </c>
+      <c r="F122" t="s">
+        <v>18</v>
+      </c>
+      <c r="G122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>39</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D123" t="s">
+        <v>19</v>
+      </c>
+      <c r="E123" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>39</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>40</v>
+      </c>
+      <c r="B125" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D125" t="s">
+        <v>19</v>
+      </c>
+      <c r="E125" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>40</v>
+      </c>
+      <c r="B126" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" t="s">
+        <v>19</v>
+      </c>
+      <c r="D126" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>51</v>
+      </c>
+      <c r="B127" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E127" t="s">
+        <v>19</v>
+      </c>
+      <c r="F127" t="s">
+        <v>20</v>
+      </c>
+      <c r="G127" s="1"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>51</v>
+      </c>
+      <c r="B128" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128" t="s">
+        <v>19</v>
+      </c>
+      <c r="E128" t="s">
+        <v>20</v>
+      </c>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>41</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D129" t="s">
+        <v>19</v>
+      </c>
+      <c r="E129" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>41</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C130" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>43</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D131" t="s">
+        <v>19</v>
+      </c>
+      <c r="E131" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>43</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132" t="s">
+        <v>19</v>
+      </c>
+      <c r="D132" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>44</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C133" t="s">
+        <v>22</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E133" t="s">
+        <v>19</v>
+      </c>
+      <c r="F133" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>44</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C134" t="s">
+        <v>22</v>
+      </c>
+      <c r="D134" t="s">
+        <v>19</v>
+      </c>
+      <c r="E134" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>45</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E135" t="s">
+        <v>19</v>
+      </c>
+      <c r="F135" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>45</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1</v>
+      </c>
+      <c r="D136" t="s">
+        <v>19</v>
+      </c>
+      <c r="E136" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>52</v>
+      </c>
+      <c r="B137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E137" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>52</v>
+      </c>
+      <c r="B138" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138" t="s">
+        <v>19</v>
+      </c>
+      <c r="E138" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>46</v>
+      </c>
+      <c r="B139" t="s">
+        <v>11</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F139" t="s">
+        <v>19</v>
+      </c>
+      <c r="G139" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>46</v>
+      </c>
+      <c r="B140" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D140" t="s">
+        <v>1</v>
+      </c>
+      <c r="E140" t="s">
+        <v>19</v>
+      </c>
+      <c r="F140" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>47</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D141" t="s">
+        <v>19</v>
+      </c>
+      <c r="E141" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>47</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>48</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E143" t="s">
+        <v>19</v>
+      </c>
+      <c r="F143" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>48</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D144" t="s">
+        <v>19</v>
+      </c>
+      <c r="E144" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>49</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E145" t="s">
+        <v>19</v>
+      </c>
+      <c r="F145" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>50</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D147" t="s">
+        <v>22</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F147" t="s">
+        <v>19</v>
+      </c>
+      <c r="G147" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>50</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D148" t="s">
+        <v>22</v>
+      </c>
+      <c r="E148" t="s">
+        <v>19</v>
+      </c>
+      <c r="F148" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>14</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>14</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>15</v>
+      </c>
+      <c r="B151" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>16</v>
+      </c>
+      <c r="B152" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>16</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>0</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>26</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>26</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>27</v>
+      </c>
+      <c r="B158" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>28</v>
+      </c>
+      <c r="B159" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>28</v>
+      </c>
+      <c r="B160" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>29</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>30</v>
+      </c>
+      <c r="B162" t="s">
+        <v>34</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>14</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>14</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>15</v>
+      </c>
+      <c r="B165" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>16</v>
+      </c>
+      <c r="B166" t="s">
+        <v>11</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>16</v>
+      </c>
+      <c r="B167" t="s">
+        <v>11</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>0</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>17</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>26</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C170" t="s">
+        <v>1</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>26</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>27</v>
+      </c>
+      <c r="B172" t="s">
+        <v>11</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>28</v>
+      </c>
+      <c r="B173" t="s">
+        <v>11</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D173" t="s">
+        <v>1</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>28</v>
+      </c>
+      <c r="B174" t="s">
+        <v>11</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>29</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>30</v>
+      </c>
+      <c r="B176" t="s">
+        <v>34</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>14</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>14</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>15</v>
+      </c>
+      <c r="B179" t="s">
+        <v>11</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>16</v>
+      </c>
+      <c r="B180" t="s">
+        <v>11</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>16</v>
+      </c>
+      <c r="B181" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>0</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>17</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>26</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>26</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>27</v>
+      </c>
+      <c r="B186" t="s">
+        <v>11</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>28</v>
+      </c>
+      <c r="B187" t="s">
+        <v>11</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>28</v>
+      </c>
+      <c r="B188" t="s">
+        <v>11</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>29</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>30</v>
+      </c>
+      <c r="B190" t="s">
+        <v>34</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>39</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>39</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>40</v>
+      </c>
+      <c r="B193" t="s">
+        <v>11</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>51</v>
+      </c>
+      <c r="B194" t="s">
+        <v>11</v>
+      </c>
+      <c r="C194" t="s">
+        <v>1</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>51</v>
+      </c>
+      <c r="B195" t="s">
+        <v>11</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>42</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>41</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>45</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C198" t="s">
+        <v>1</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>45</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>52</v>
+      </c>
+      <c r="B200" t="s">
+        <v>11</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>46</v>
+      </c>
+      <c r="B201" t="s">
+        <v>11</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D201" t="s">
+        <v>1</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>46</v>
+      </c>
+      <c r="B202" t="s">
+        <v>11</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>47</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>48</v>
+      </c>
+      <c r="B204" t="s">
+        <v>34</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>39</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>39</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>40</v>
+      </c>
+      <c r="B207" t="s">
+        <v>11</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>51</v>
+      </c>
+      <c r="B208" t="s">
+        <v>11</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>51</v>
+      </c>
+      <c r="B209" t="s">
+        <v>11</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>42</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>41</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>45</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>45</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>52</v>
+      </c>
+      <c r="B214" t="s">
+        <v>11</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>46</v>
+      </c>
+      <c r="B215" t="s">
+        <v>11</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D215" t="s">
+        <v>1</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>46</v>
+      </c>
+      <c r="B216" t="s">
+        <v>11</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>47</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>48</v>
+      </c>
+      <c r="B218" t="s">
+        <v>34</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>39</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>39</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>40</v>
+      </c>
+      <c r="B221" t="s">
+        <v>11</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>51</v>
+      </c>
+      <c r="B222" t="s">
+        <v>11</v>
+      </c>
+      <c r="C222" t="s">
+        <v>1</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>51</v>
+      </c>
+      <c r="B223" t="s">
+        <v>11</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>42</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>41</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>45</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C226" t="s">
+        <v>1</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>45</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>52</v>
+      </c>
+      <c r="B228" t="s">
+        <v>11</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>46</v>
+      </c>
+      <c r="B229" t="s">
+        <v>11</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D229" t="s">
+        <v>1</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>46</v>
+      </c>
+      <c r="B230" t="s">
+        <v>11</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>47</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>48</v>
+      </c>
+      <c r="B232" t="s">
+        <v>34</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35202B10-EF9C-E146-B10F-6C6531951459}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
- fix laplace and feature selection
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9D303D-1A32-3040-AFB0-50F44140D94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F67065-6F4F-AF41-84D0-9B54A9758D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio4" sheetId="4" r:id="rId3"/>
-    <sheet name="Foglio3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2271" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="67">
   <si>
     <t>ds</t>
   </si>
@@ -1494,10 +1493,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:H232"/>
+  <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:XFD107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3257,333 +3256,357 @@
       <c r="A93" t="s">
         <v>42</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>6</v>
+      <c r="B93" t="s">
+        <v>38</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D93" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B94" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D94" t="s">
-        <v>5</v>
-      </c>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>42</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>19</v>
+        <v>40</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E95" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D95" t="s">
+        <v>19</v>
+      </c>
+      <c r="E95" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B96" t="s">
-        <v>38</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E96" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
+        <v>20</v>
+      </c>
+      <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>39</v>
-      </c>
-      <c r="B97" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" t="s">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D97" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E97" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>39</v>
-      </c>
-      <c r="B98" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D98" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E98" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>40</v>
-      </c>
-      <c r="B99" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E99" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>40</v>
-      </c>
-      <c r="B100" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C100" t="s">
-        <v>25</v>
-      </c>
-      <c r="D100" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E100" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
-      </c>
-      <c r="C101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D101" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E101" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B102" t="s">
-        <v>34</v>
-      </c>
-      <c r="C102" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D102" t="s">
-        <v>18</v>
-      </c>
-      <c r="E102" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F102" t="s">
+        <v>19</v>
+      </c>
+      <c r="G102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>41</v>
-      </c>
-      <c r="B103" t="s">
-        <v>6</v>
-      </c>
-      <c r="C103" t="s">
-        <v>18</v>
+        <v>47</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D103" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="E103" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>41</v>
-      </c>
-      <c r="B104" t="s">
-        <v>25</v>
-      </c>
-      <c r="C104" t="s">
-        <v>18</v>
-      </c>
-      <c r="D104" t="s">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E104" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C105" t="s">
-        <v>6</v>
-      </c>
-      <c r="D105" t="s">
-        <v>18</v>
+      <c r="D105" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E105" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="F105" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" t="s">
         <v>22</v>
       </c>
-      <c r="C106" t="s">
-        <v>25</v>
-      </c>
-      <c r="D106" t="s">
-        <v>18</v>
-      </c>
-      <c r="E106" t="s">
-        <v>5</v>
+      <c r="E106" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F106" t="s">
+        <v>19</v>
+      </c>
+      <c r="G106" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>44</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C107" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D107" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E107" t="s">
-        <v>18</v>
-      </c>
-      <c r="F107" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>44</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C108" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="B108" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D108" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E108" t="s">
-        <v>18</v>
-      </c>
-      <c r="F108" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>45</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
-      <c r="D109" t="s">
-        <v>6</v>
+      <c r="D109" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E109" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F109" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C110" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D110" t="s">
-        <v>25</v>
-      </c>
-      <c r="E110" t="s">
-        <v>18</v>
-      </c>
-      <c r="F110" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B111" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D111" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E111" t="s">
-        <v>6</v>
-      </c>
-      <c r="F111" t="s">
-        <v>18</v>
-      </c>
-      <c r="G111" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B112" t="s">
         <v>11</v>
@@ -3592,33 +3615,30 @@
         <v>33</v>
       </c>
       <c r="D112" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E112" t="s">
-        <v>25</v>
-      </c>
-      <c r="F112" t="s">
-        <v>18</v>
-      </c>
-      <c r="G112" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>47</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="B113" t="s">
+        <v>11</v>
       </c>
       <c r="C113" t="s">
-        <v>6</v>
-      </c>
-      <c r="D113" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E113" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="F113" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -3629,1051 +3649,448 @@
         <v>33</v>
       </c>
       <c r="C114" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D114" t="s">
-        <v>18</v>
-      </c>
-      <c r="E114" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>48</v>
-      </c>
-      <c r="B115" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D115" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E115" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F115" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>48</v>
-      </c>
-      <c r="B116" t="s">
-        <v>34</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C116" t="s">
+        <v>22</v>
       </c>
       <c r="D116" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E116" t="s">
-        <v>18</v>
-      </c>
-      <c r="F116" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>48</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C117" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E117" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="F117" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>48</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C118" t="s">
-        <v>25</v>
-      </c>
-      <c r="D118" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="B118" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E118" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="F118" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>49</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D119" t="s">
-        <v>6</v>
-      </c>
-      <c r="E119" t="s">
-        <v>18</v>
+        <v>59</v>
+      </c>
+      <c r="B119" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="F119" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G119" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D120" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E120" t="s">
-        <v>18</v>
-      </c>
-      <c r="F120" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>50</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>24</v>
+        <v>61</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D121" t="s">
-        <v>22</v>
+      <c r="D121" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E121" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="F121" t="s">
-        <v>18</v>
-      </c>
-      <c r="G121" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>50</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>24</v>
+        <v>62</v>
+      </c>
+      <c r="B122" t="s">
+        <v>11</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D122" t="s">
-        <v>22</v>
+      <c r="D122" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E122" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F122" t="s">
-        <v>18</v>
-      </c>
-      <c r="G122" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B123" t="s">
-        <v>1</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D123" t="s">
-        <v>19</v>
-      </c>
-      <c r="E123" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F123" t="s">
+        <v>35</v>
+      </c>
+      <c r="G123" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>39</v>
-      </c>
-      <c r="B124" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" t="s">
-        <v>19</v>
+        <v>64</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D124" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="E124" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>40</v>
-      </c>
-      <c r="B125" t="s">
-        <v>11</v>
+        <v>65</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D125" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E125" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="F125" t="s">
+        <v>35</v>
+      </c>
+      <c r="G125" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>40</v>
-      </c>
-      <c r="B126" t="s">
-        <v>11</v>
-      </c>
-      <c r="C126" t="s">
-        <v>19</v>
+        <v>66</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D126" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="E126" t="s">
+        <v>35</v>
+      </c>
+      <c r="F126" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>51</v>
-      </c>
-      <c r="B127" t="s">
-        <v>11</v>
-      </c>
-      <c r="C127" t="s">
-        <v>1</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E127" t="s">
-        <v>19</v>
-      </c>
-      <c r="F127" t="s">
-        <v>20</v>
-      </c>
-      <c r="G127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>51</v>
-      </c>
-      <c r="B128" t="s">
-        <v>11</v>
-      </c>
-      <c r="C128" t="s">
-        <v>1</v>
-      </c>
-      <c r="D128" t="s">
-        <v>19</v>
-      </c>
-      <c r="E128" t="s">
-        <v>20</v>
-      </c>
-      <c r="F128" s="1"/>
-      <c r="G128" s="1"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>41</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D129" t="s">
-        <v>19</v>
-      </c>
-      <c r="E129" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>41</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C130" t="s">
-        <v>19</v>
-      </c>
-      <c r="D130" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>43</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D131" t="s">
-        <v>19</v>
-      </c>
-      <c r="E131" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>43</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C132" t="s">
-        <v>19</v>
-      </c>
-      <c r="D132" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>44</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C133" t="s">
-        <v>22</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E133" t="s">
-        <v>19</v>
-      </c>
-      <c r="F133" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>44</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C134" t="s">
-        <v>22</v>
-      </c>
-      <c r="D134" t="s">
-        <v>19</v>
-      </c>
-      <c r="E134" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>45</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C135" t="s">
-        <v>1</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E135" t="s">
-        <v>19</v>
-      </c>
-      <c r="F135" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>45</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C136" t="s">
-        <v>1</v>
-      </c>
-      <c r="D136" t="s">
-        <v>19</v>
-      </c>
-      <c r="E136" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>52</v>
-      </c>
-      <c r="B137" t="s">
-        <v>11</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E137" t="s">
-        <v>19</v>
-      </c>
-      <c r="F137" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>52</v>
-      </c>
-      <c r="B138" t="s">
-        <v>11</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D138" t="s">
-        <v>19</v>
-      </c>
-      <c r="E138" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>46</v>
-      </c>
-      <c r="B139" t="s">
-        <v>11</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D139" t="s">
-        <v>1</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F139" t="s">
-        <v>19</v>
-      </c>
-      <c r="G139" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>46</v>
-      </c>
-      <c r="B140" t="s">
-        <v>11</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D140" t="s">
-        <v>1</v>
-      </c>
-      <c r="E140" t="s">
-        <v>19</v>
-      </c>
-      <c r="F140" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>47</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D141" t="s">
-        <v>19</v>
-      </c>
-      <c r="E141" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>47</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>48</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E143" t="s">
-        <v>19</v>
-      </c>
-      <c r="F143" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>48</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D144" t="s">
-        <v>19</v>
-      </c>
-      <c r="E144" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>49</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E145" t="s">
-        <v>19</v>
-      </c>
-      <c r="F145" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F146" s="1"/>
-      <c r="G146" s="1"/>
-      <c r="H146" s="1"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>50</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D147" t="s">
-        <v>22</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F147" t="s">
-        <v>19</v>
-      </c>
-      <c r="G147" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>50</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D148" t="s">
-        <v>22</v>
-      </c>
-      <c r="E148" t="s">
-        <v>19</v>
-      </c>
-      <c r="F148" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>26</v>
-      </c>
-      <c r="B149" t="s">
-        <v>1</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D149" t="s">
-        <v>35</v>
-      </c>
-      <c r="E149" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>27</v>
-      </c>
-      <c r="B150" t="s">
-        <v>11</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D150" t="s">
-        <v>35</v>
-      </c>
-      <c r="E150" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>28</v>
-      </c>
-      <c r="B151" t="s">
-        <v>11</v>
-      </c>
-      <c r="C151" t="s">
-        <v>1</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E151" t="s">
-        <v>35</v>
-      </c>
-      <c r="F151" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>29</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C152" t="s">
-        <v>35</v>
-      </c>
-      <c r="D152" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>45</v>
-      </c>
-      <c r="B153" t="s">
-        <v>1</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D153" t="s">
-        <v>35</v>
-      </c>
-      <c r="E153" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>52</v>
-      </c>
-      <c r="B154" t="s">
-        <v>11</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D154" t="s">
-        <v>35</v>
-      </c>
-      <c r="E154" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>46</v>
-      </c>
-      <c r="B155" t="s">
-        <v>11</v>
-      </c>
-      <c r="C155" t="s">
-        <v>1</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E155" t="s">
-        <v>35</v>
-      </c>
-      <c r="F155" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>47</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C156" t="s">
-        <v>35</v>
-      </c>
-      <c r="D156" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
-        <v>50</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D157" t="s">
-        <v>22</v>
-      </c>
-      <c r="E157" t="s">
-        <v>35</v>
-      </c>
-      <c r="F157" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>49</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C158" t="s">
-        <v>22</v>
-      </c>
-      <c r="D158" t="s">
-        <v>35</v>
-      </c>
-      <c r="E158" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>57</v>
-      </c>
-      <c r="B159" t="s">
-        <v>1</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E159" t="s">
-        <v>35</v>
-      </c>
-      <c r="F159" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>58</v>
-      </c>
-      <c r="B160" t="s">
-        <v>11</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E160" t="s">
-        <v>35</v>
-      </c>
-      <c r="F160" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>59</v>
-      </c>
-      <c r="B161" t="s">
-        <v>11</v>
-      </c>
-      <c r="C161" t="s">
-        <v>1</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F161" t="s">
-        <v>35</v>
-      </c>
-      <c r="G161" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>60</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D162" t="s">
-        <v>35</v>
-      </c>
-      <c r="E162" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>61</v>
-      </c>
-      <c r="B163" t="s">
-        <v>1</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E163" t="s">
-        <v>35</v>
-      </c>
-      <c r="F163" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>62</v>
-      </c>
-      <c r="B164" t="s">
-        <v>11</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E164" t="s">
-        <v>35</v>
-      </c>
-      <c r="F164" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>63</v>
-      </c>
-      <c r="B165" t="s">
-        <v>11</v>
-      </c>
-      <c r="C165" t="s">
-        <v>1</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F165" t="s">
-        <v>35</v>
-      </c>
-      <c r="G165" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>64</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D166" t="s">
-        <v>35</v>
-      </c>
-      <c r="E166" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>65</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E167" t="s">
-        <v>22</v>
-      </c>
-      <c r="F167" t="s">
-        <v>35</v>
-      </c>
-      <c r="G167" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>66</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D168" t="s">
-        <v>22</v>
-      </c>
-      <c r="E168" t="s">
-        <v>35</v>
-      </c>
-      <c r="F168" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B128" s="1"/>
+      <c r="D128" s="1"/>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C131" s="1"/>
+      <c r="E131" s="1"/>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C137" s="1"/>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D138" s="1"/>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B142" s="1"/>
+      <c r="D142" s="1"/>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C145" s="1"/>
+      <c r="E145" s="1"/>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C151" s="1"/>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D152" s="1"/>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B156" s="1"/>
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+    </row>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C159" s="1"/>
+      <c r="E159" s="1"/>
+    </row>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D166" s="1"/>
+    </row>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+    </row>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B170" s="1"/>
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C173" s="1"/>
       <c r="E173" s="1"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
     </row>
@@ -4731,171 +4148,6 @@
     <row r="190" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
-    </row>
-    <row r="191" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B191" s="1"/>
-      <c r="C191" s="1"/>
-    </row>
-    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B192" s="1"/>
-      <c r="C192" s="1"/>
-    </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C193" s="1"/>
-    </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D194" s="1"/>
-    </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C195" s="1"/>
-      <c r="D195" s="1"/>
-    </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B196" s="1"/>
-    </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B197" s="1"/>
-      <c r="C197" s="1"/>
-    </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B198" s="1"/>
-      <c r="D198" s="1"/>
-    </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B199" s="1"/>
-      <c r="C199" s="1"/>
-      <c r="D199" s="1"/>
-    </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C200" s="1"/>
-      <c r="D200" s="1"/>
-    </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C201" s="1"/>
-      <c r="E201" s="1"/>
-    </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C202" s="1"/>
-      <c r="D202" s="1"/>
-      <c r="E202" s="1"/>
-    </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
-    </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C204" s="1"/>
-      <c r="D204" s="1"/>
-    </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B205" s="1"/>
-      <c r="C205" s="1"/>
-    </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B206" s="1"/>
-      <c r="C206" s="1"/>
-    </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C207" s="1"/>
-    </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D208" s="1"/>
-    </row>
-    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C209" s="1"/>
-      <c r="D209" s="1"/>
-    </row>
-    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B210" s="1"/>
-    </row>
-    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B211" s="1"/>
-      <c r="C211" s="1"/>
-    </row>
-    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B212" s="1"/>
-      <c r="D212" s="1"/>
-    </row>
-    <row r="213" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B213" s="1"/>
-      <c r="C213" s="1"/>
-      <c r="D213" s="1"/>
-    </row>
-    <row r="214" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C214" s="1"/>
-      <c r="D214" s="1"/>
-    </row>
-    <row r="215" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C215" s="1"/>
-      <c r="E215" s="1"/>
-    </row>
-    <row r="216" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C216" s="1"/>
-      <c r="D216" s="1"/>
-      <c r="E216" s="1"/>
-    </row>
-    <row r="217" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
-    </row>
-    <row r="218" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C218" s="1"/>
-      <c r="D218" s="1"/>
-    </row>
-    <row r="219" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
-    </row>
-    <row r="220" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B220" s="1"/>
-      <c r="C220" s="1"/>
-    </row>
-    <row r="221" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C221" s="1"/>
-    </row>
-    <row r="222" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D222" s="1"/>
-    </row>
-    <row r="223" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C223" s="1"/>
-      <c r="D223" s="1"/>
-    </row>
-    <row r="224" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B224" s="1"/>
-    </row>
-    <row r="225" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B225" s="1"/>
-      <c r="C225" s="1"/>
-    </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B226" s="1"/>
-      <c r="D226" s="1"/>
-    </row>
-    <row r="227" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B227" s="1"/>
-      <c r="C227" s="1"/>
-      <c r="D227" s="1"/>
-    </row>
-    <row r="228" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C228" s="1"/>
-      <c r="D228" s="1"/>
-    </row>
-    <row r="229" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C229" s="1"/>
-      <c r="E229" s="1"/>
-    </row>
-    <row r="230" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C230" s="1"/>
-      <c r="D230" s="1"/>
-      <c r="E230" s="1"/>
-    </row>
-    <row r="231" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B231" s="1"/>
-      <c r="C231" s="1"/>
-    </row>
-    <row r="232" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C232" s="1"/>
-      <c r="D232" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4906,8 +4158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D2990A-F429-0248-9892-0EF6030E3150}">
   <dimension ref="A1:H232"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="A212" sqref="A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8730,16 +7982,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35202B10-EF9C-E146-B10F-6C6531951459}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- add regression - add cross validation - modified classification - modified roc curve
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5634479-8FC7-FF4A-8755-3C20BE5D0282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0559AB-7EB1-5442-85ED-0E4F28586001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
+    <workbookView xWindow="4020" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio4" sheetId="4" r:id="rId3"/>
     <sheet name="Foglio3" sheetId="5" r:id="rId4"/>
+    <sheet name="Foglio5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="74">
   <si>
     <t>ds</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>moreFeatures, hasLabel</t>
+  </si>
+  <si>
+    <t>kFold</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1518,7 @@
   <dimension ref="A1:H190"/>
   <sheetViews>
     <sheetView topLeftCell="A103" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122:E122"/>
+      <selection activeCell="A123" sqref="A123:G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4305,7 +4308,7 @@
   <dimension ref="A1:H232"/>
   <sheetViews>
     <sheetView topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212"/>
+      <selection activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8134,8 +8137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FAA623-A1BD-4D43-86F2-BAAF15CFDB2B}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8239,4 +8242,160 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE1144B-1EE3-8F43-A85B-2666765C475A}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- todo: classifier fix
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54580081-1423-BB4B-B89E-062F97410F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233B256-B18C-6641-A7F8-A210024BB28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2203" uniqueCount="76">
   <si>
     <t>ds</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>kFold</t>
+  </si>
+  <si>
+    <t>missingValuesFill</t>
   </si>
 </sst>
 </file>
@@ -1520,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
   <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:A66"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="99" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1537,8 +1540,8 @@
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1554,8 +1557,8 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1571,8 +1574,8 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1636,8 +1639,8 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -1656,8 +1659,8 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
-        <v>1</v>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -1676,8 +1679,8 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>1</v>
+      <c r="C9" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -1922,8 +1925,8 @@
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C24" t="s">
-        <v>1</v>
+      <c r="C24" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1942,8 +1945,8 @@
       <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
-        <v>1</v>
+      <c r="C25" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1962,8 +1965,8 @@
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" t="s">
-        <v>1</v>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D26" t="s">
         <v>19</v>
@@ -1976,8 +1979,8 @@
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>1</v>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
@@ -2067,8 +2070,8 @@
       <c r="C32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D32" t="s">
-        <v>1</v>
+      <c r="D32" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -2090,8 +2093,8 @@
       <c r="C33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D33" t="s">
-        <v>1</v>
+      <c r="D33" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
@@ -2113,8 +2116,8 @@
       <c r="C34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D34" t="s">
-        <v>1</v>
+      <c r="D34" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -2130,8 +2133,8 @@
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C35" t="s">
-        <v>1</v>
+      <c r="C35" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D35" t="s">
         <v>19</v>
@@ -2457,9 +2460,12 @@
         <v>33</v>
       </c>
       <c r="D53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" t="s">
         <v>35</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2474,9 +2480,12 @@
         <v>33</v>
       </c>
       <c r="D54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" t="s">
         <v>35</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2491,9 +2500,12 @@
         <v>33</v>
       </c>
       <c r="D55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" t="s">
         <v>35</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2511,9 +2523,12 @@
         <v>22</v>
       </c>
       <c r="E56" t="s">
+        <v>74</v>
+      </c>
+      <c r="F56" t="s">
         <v>35</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2531,9 +2546,12 @@
         <v>22</v>
       </c>
       <c r="E57" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" t="s">
         <v>35</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2551,9 +2569,12 @@
         <v>22</v>
       </c>
       <c r="E58" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" t="s">
         <v>35</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2571,9 +2592,12 @@
         <v>33</v>
       </c>
       <c r="E59" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" t="s">
         <v>35</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="G59" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2591,9 +2615,12 @@
         <v>33</v>
       </c>
       <c r="E60" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" t="s">
         <v>35</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2611,9 +2638,12 @@
         <v>33</v>
       </c>
       <c r="E61" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" t="s">
         <v>35</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="G61" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2631,9 +2661,12 @@
         <v>22</v>
       </c>
       <c r="E62" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" t="s">
         <v>35</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="G62" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2651,9 +2684,12 @@
         <v>22</v>
       </c>
       <c r="E63" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="G63" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2671,9 +2707,12 @@
         <v>22</v>
       </c>
       <c r="E64" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" t="s">
         <v>35</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="G64" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2682,7 +2721,7 @@
         <v>39</v>
       </c>
       <c r="B65" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
         <v>38</v>
@@ -2702,7 +2741,7 @@
         <v>39</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
@@ -3014,8 +3053,8 @@
       <c r="B81" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C81" t="s">
-        <v>1</v>
+      <c r="C81" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D81" t="s">
         <v>38</v>
@@ -3037,8 +3076,8 @@
       <c r="B82" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C82" t="s">
-        <v>1</v>
+      <c r="C82" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D82" t="s">
         <v>38</v>
@@ -3064,7 +3103,7 @@
         <v>33</v>
       </c>
       <c r="D83" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="E83" t="s">
         <v>38</v>
@@ -3090,7 +3129,7 @@
         <v>33</v>
       </c>
       <c r="D84" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="E84" t="s">
         <v>38</v>
@@ -3349,7 +3388,7 @@
         <v>39</v>
       </c>
       <c r="B96" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>38</v>
@@ -3386,7 +3425,7 @@
         <v>11</v>
       </c>
       <c r="C98" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>38</v>
@@ -3460,8 +3499,8 @@
       <c r="B102" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C102" t="s">
-        <v>1</v>
+      <c r="C102" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>38</v>
@@ -3504,7 +3543,7 @@
         <v>33</v>
       </c>
       <c r="D104" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>38</v>
@@ -3601,15 +3640,18 @@
         <v>26</v>
       </c>
       <c r="B109" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D109" t="s">
+        <v>74</v>
+      </c>
+      <c r="E109" t="s">
         <v>35</v>
       </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3624,9 +3666,12 @@
         <v>33</v>
       </c>
       <c r="D110" t="s">
+        <v>74</v>
+      </c>
+      <c r="E110" t="s">
         <v>35</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3637,16 +3682,19 @@
       <c r="B111" t="s">
         <v>11</v>
       </c>
-      <c r="C111" t="s">
-        <v>1</v>
+      <c r="C111" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E111" t="s">
+        <v>74</v>
+      </c>
+      <c r="F111" t="s">
         <v>35</v>
       </c>
-      <c r="F111" t="s">
+      <c r="G111" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3658,30 +3706,36 @@
         <v>33</v>
       </c>
       <c r="C112" t="s">
+        <v>74</v>
+      </c>
+      <c r="D112" t="s">
         <v>35</v>
       </c>
-      <c r="D112" t="s">
+      <c r="E112" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>45</v>
       </c>
-      <c r="B113" t="s">
-        <v>1</v>
+      <c r="B113" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D113" t="s">
+        <v>74</v>
+      </c>
+      <c r="E113" t="s">
         <v>35</v>
       </c>
-      <c r="E113" t="s">
+      <c r="F113" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>52</v>
       </c>
@@ -3692,33 +3746,39 @@
         <v>33</v>
       </c>
       <c r="D114" t="s">
+        <v>74</v>
+      </c>
+      <c r="E114" t="s">
         <v>35</v>
       </c>
-      <c r="E114" t="s">
+      <c r="F114" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>46</v>
       </c>
       <c r="B115" t="s">
         <v>11</v>
       </c>
-      <c r="C115" t="s">
-        <v>1</v>
+      <c r="C115" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E115" t="s">
+        <v>74</v>
+      </c>
+      <c r="F115" t="s">
         <v>35</v>
       </c>
-      <c r="F115" t="s">
+      <c r="G115" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>47</v>
       </c>
@@ -3726,13 +3786,16 @@
         <v>33</v>
       </c>
       <c r="C116" t="s">
+        <v>74</v>
+      </c>
+      <c r="D116" t="s">
         <v>35</v>
       </c>
-      <c r="D116" t="s">
+      <c r="E116" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>50</v>
       </c>
@@ -3746,13 +3809,16 @@
         <v>22</v>
       </c>
       <c r="E117" t="s">
+        <v>74</v>
+      </c>
+      <c r="F117" t="s">
         <v>35</v>
       </c>
-      <c r="F117" t="s">
+      <c r="G117" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>49</v>
       </c>
@@ -3763,18 +3829,21 @@
         <v>22</v>
       </c>
       <c r="D118" t="s">
+        <v>74</v>
+      </c>
+      <c r="E118" t="s">
         <v>35</v>
       </c>
-      <c r="E118" t="s">
+      <c r="F118" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>57</v>
       </c>
-      <c r="B119" t="s">
-        <v>1</v>
+      <c r="B119" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>33</v>
@@ -3783,13 +3852,16 @@
         <v>34</v>
       </c>
       <c r="E119" t="s">
+        <v>74</v>
+      </c>
+      <c r="F119" t="s">
         <v>35</v>
       </c>
-      <c r="F119" t="s">
+      <c r="G119" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>58</v>
       </c>
@@ -3803,21 +3875,24 @@
         <v>34</v>
       </c>
       <c r="E120" t="s">
+        <v>74</v>
+      </c>
+      <c r="F120" t="s">
         <v>35</v>
       </c>
-      <c r="F120" t="s">
+      <c r="G120" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>59</v>
       </c>
       <c r="B121" t="s">
         <v>11</v>
       </c>
-      <c r="C121" t="s">
-        <v>1</v>
+      <c r="C121" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>33</v>
@@ -3826,13 +3901,16 @@
         <v>34</v>
       </c>
       <c r="F121" t="s">
+        <v>74</v>
+      </c>
+      <c r="G121" t="s">
         <v>35</v>
       </c>
-      <c r="G121" t="s">
+      <c r="H121" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>60</v>
       </c>
@@ -3843,18 +3921,21 @@
         <v>34</v>
       </c>
       <c r="D122" t="s">
+        <v>74</v>
+      </c>
+      <c r="E122" t="s">
         <v>35</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>61</v>
       </c>
-      <c r="B123" t="s">
-        <v>1</v>
+      <c r="B123" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>33</v>
@@ -3863,13 +3944,16 @@
         <v>34</v>
       </c>
       <c r="E123" t="s">
+        <v>74</v>
+      </c>
+      <c r="F123" t="s">
         <v>35</v>
       </c>
-      <c r="F123" t="s">
+      <c r="G123" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>62</v>
       </c>
@@ -3883,21 +3967,24 @@
         <v>34</v>
       </c>
       <c r="E124" t="s">
+        <v>74</v>
+      </c>
+      <c r="F124" t="s">
         <v>35</v>
       </c>
-      <c r="F124" t="s">
+      <c r="G124" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>63</v>
       </c>
       <c r="B125" t="s">
         <v>11</v>
       </c>
-      <c r="C125" t="s">
-        <v>1</v>
+      <c r="C125" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>33</v>
@@ -3906,13 +3993,16 @@
         <v>34</v>
       </c>
       <c r="F125" t="s">
+        <v>74</v>
+      </c>
+      <c r="G125" t="s">
         <v>35</v>
       </c>
-      <c r="G125" t="s">
+      <c r="H125" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>64</v>
       </c>
@@ -3923,13 +4013,16 @@
         <v>34</v>
       </c>
       <c r="D126" t="s">
+        <v>74</v>
+      </c>
+      <c r="E126" t="s">
         <v>35</v>
       </c>
-      <c r="E126" t="s">
+      <c r="F126" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>65</v>
       </c>
@@ -3946,13 +4039,16 @@
         <v>22</v>
       </c>
       <c r="F127" t="s">
+        <v>74</v>
+      </c>
+      <c r="G127" t="s">
         <v>35</v>
       </c>
-      <c r="G127" t="s">
+      <c r="H127" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>66</v>
       </c>
@@ -3966,9 +4062,12 @@
         <v>22</v>
       </c>
       <c r="E128" t="s">
+        <v>74</v>
+      </c>
+      <c r="F128" t="s">
         <v>35</v>
       </c>
-      <c r="F128" t="s">
+      <c r="G128" t="s">
         <v>56</v>
       </c>
     </row>
@@ -8252,7 +8351,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
- fix classifier - add classifiers - add outliers detection - add sentences in training data - add plot - modified kb - add feature importance class
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233B256-B18C-6641-A7F8-A210024BB28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3482EA-D1B6-C244-8ECC-6825E0BA317E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
+    <workbookView xWindow="660" yWindow="2280" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2203" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2537" uniqueCount="90">
   <si>
     <t>ds</t>
   </si>
@@ -253,12 +253,6 @@
     <t>kMeans</t>
   </si>
   <si>
-    <t>logisticRegression</t>
-  </si>
-  <si>
-    <t>moreFeatures, hasLabel</t>
-  </si>
-  <si>
     <t>crossValidation</t>
   </si>
   <si>
@@ -266,6 +260,54 @@
   </si>
   <si>
     <t>missingValuesFill</t>
+  </si>
+  <si>
+    <t>missingValuesHandle</t>
+  </si>
+  <si>
+    <t>outliersDetection</t>
+  </si>
+  <si>
+    <t>missingValues, outliers</t>
+  </si>
+  <si>
+    <t>missingValues, outliers, moreFeatures</t>
+  </si>
+  <si>
+    <t>missingValues, outliers, moreFeatures, hasLabel</t>
+  </si>
+  <si>
+    <t>missingValues, outliers, hasLabel</t>
+  </si>
+  <si>
+    <t>categorical, onlyCategorical, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>missingValues, onlyCategorical, categorical, hasLabel, moreFeatures</t>
+  </si>
+  <si>
+    <t>onlyCategorical, hasLabel, moreFeatures, outliers,categorical</t>
+  </si>
+  <si>
+    <t>moreFeatures, categorical, onlyCategorical</t>
+  </si>
+  <si>
+    <t>missingValues, outliers, categorical</t>
+  </si>
+  <si>
+    <t>missingValues, outliers, moreFeatures, categorical</t>
+  </si>
+  <si>
+    <t>missingValues, outliers, moreFeatures, hasLabel, categorical</t>
+  </si>
+  <si>
+    <t>missingValues, outliers, hasLabel, categorical</t>
+  </si>
+  <si>
+    <t>featureImportance</t>
+  </si>
+  <si>
+    <t>featureImportancePlot</t>
   </si>
 </sst>
 </file>
@@ -1521,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:H190"/>
+  <dimension ref="A1:I222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1534,6 +1576,8 @@
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1541,7 +1585,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1558,7 +1602,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1575,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1640,7 +1684,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -1660,7 +1704,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -1680,7 +1724,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -1866,7 +1910,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
@@ -1886,7 +1930,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -1906,7 +1950,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
@@ -1926,7 +1970,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1946,7 +1990,7 @@
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1966,7 +2010,7 @@
         <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
         <v>19</v>
@@ -1980,7 +2024,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
@@ -2071,7 +2115,7 @@
         <v>33</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -2094,7 +2138,7 @@
         <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
@@ -2117,7 +2161,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -2134,7 +2178,7 @@
         <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" t="s">
         <v>19</v>
@@ -2460,7 +2504,7 @@
         <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E53" t="s">
         <v>35</v>
@@ -2480,7 +2524,7 @@
         <v>33</v>
       </c>
       <c r="D54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E54" t="s">
         <v>35</v>
@@ -2500,7 +2544,7 @@
         <v>33</v>
       </c>
       <c r="D55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E55" t="s">
         <v>35</v>
@@ -2511,7 +2555,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>24</v>
@@ -2519,22 +2563,22 @@
       <c r="C56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>22</v>
+      <c r="D56" t="s">
+        <v>72</v>
       </c>
       <c r="E56" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="F56" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="G56" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>24</v>
@@ -2542,22 +2586,22 @@
       <c r="C57" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>22</v>
+      <c r="D57" t="s">
+        <v>72</v>
       </c>
       <c r="E57" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="F57" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="G57" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>24</v>
@@ -2565,34 +2609,34 @@
       <c r="C58" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>22</v>
+      <c r="D58" t="s">
+        <v>72</v>
       </c>
       <c r="E58" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="F58" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="G58" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C59" t="s">
-        <v>11</v>
+      <c r="C59" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F59" t="s">
         <v>35</v>
@@ -2603,7 +2647,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>24</v>
@@ -2612,10 +2656,10 @@
         <v>33</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F60" t="s">
         <v>35</v>
@@ -2626,7 +2670,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>24</v>
@@ -2635,10 +2679,10 @@
         <v>33</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E61" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F61" t="s">
         <v>35</v>
@@ -2649,19 +2693,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>33</v>
+      <c r="C62" t="s">
+        <v>11</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F62" t="s">
         <v>35</v>
@@ -2672,7 +2716,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>24</v>
@@ -2681,10 +2725,10 @@
         <v>33</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F63" t="s">
         <v>35</v>
@@ -2695,7 +2739,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>24</v>
@@ -2704,10 +2748,10 @@
         <v>33</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F64" t="s">
         <v>35</v>
@@ -2718,398 +2762,453 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>39</v>
-      </c>
-      <c r="B65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>38</v>
-      </c>
-      <c r="D65" t="s">
-        <v>6</v>
+        <v>36</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E65" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F65" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G65" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>39</v>
-      </c>
-      <c r="B66" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" t="s">
-        <v>38</v>
-      </c>
-      <c r="D66" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E66" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F66" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G66" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>40</v>
-      </c>
-      <c r="B67" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
+        <v>36</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E67" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F67" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G67" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>40</v>
-      </c>
-      <c r="B68" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" t="s">
-        <v>38</v>
-      </c>
-      <c r="D68" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E68" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F68" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G68" t="s">
+        <v>88</v>
+      </c>
+      <c r="H68" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>42</v>
-      </c>
-      <c r="B69" t="s">
-        <v>38</v>
-      </c>
-      <c r="C69" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E69" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="F69" t="s">
+        <v>35</v>
+      </c>
+      <c r="G69" t="s">
+        <v>88</v>
+      </c>
+      <c r="H69" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>42</v>
-      </c>
-      <c r="B70" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" t="s">
-        <v>6</v>
+        <v>36</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E70" t="s">
-        <v>5</v>
-      </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="F70" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" t="s">
+        <v>88</v>
+      </c>
+      <c r="H70" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B71" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>38</v>
-      </c>
-      <c r="D71" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E71" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F71" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G71" t="s">
+        <v>88</v>
+      </c>
+      <c r="H71" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>41</v>
-      </c>
-      <c r="B72" t="s">
-        <v>34</v>
-      </c>
-      <c r="C72" t="s">
-        <v>38</v>
-      </c>
-      <c r="D72" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E72" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F72" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G72" t="s">
+        <v>88</v>
+      </c>
+      <c r="H72" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>41</v>
-      </c>
-      <c r="B73" t="s">
-        <v>38</v>
-      </c>
-      <c r="C73" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" t="s">
-        <v>18</v>
+        <v>37</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E73" t="s">
-        <v>5</v>
+        <v>72</v>
+      </c>
+      <c r="F73" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" t="s">
+        <v>88</v>
+      </c>
+      <c r="H73" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>41</v>
-      </c>
-      <c r="B74" t="s">
-        <v>38</v>
-      </c>
-      <c r="C74" t="s">
-        <v>25</v>
-      </c>
-      <c r="D74" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E74" t="s">
-        <v>5</v>
+        <v>72</v>
+      </c>
+      <c r="F74" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" t="s">
+        <v>88</v>
+      </c>
+      <c r="H74" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C75" t="s">
-        <v>38</v>
-      </c>
-      <c r="D75" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E75" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F75" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G75" t="s">
+        <v>88</v>
+      </c>
+      <c r="H75" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C76" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E76" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F76" t="s">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="G76" t="s">
+        <v>88</v>
+      </c>
+      <c r="H76" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>44</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D77" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E77" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F77" t="s">
-        <v>18</v>
-      </c>
-      <c r="G77" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>44</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="B78" t="s">
+        <v>74</v>
       </c>
       <c r="C78" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D78" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E78" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F78" t="s">
-        <v>18</v>
-      </c>
-      <c r="G78" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>69</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="B79" t="s">
+        <v>11</v>
       </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D79" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E79" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F79" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" t="s">
-        <v>18</v>
-      </c>
-      <c r="H79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>69</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D80" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E80" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F80" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="G80" t="s">
-        <v>18</v>
-      </c>
-      <c r="H80" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>45</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" t="s">
         <v>38</v>
       </c>
+      <c r="C81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E81" t="s">
-        <v>6</v>
-      </c>
-      <c r="F81" t="s">
-        <v>18</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F81" s="1"/>
       <c r="G81" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>45</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" t="s">
         <v>38</v>
       </c>
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E82" t="s">
-        <v>25</v>
-      </c>
-      <c r="F82" t="s">
-        <v>18</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F82" s="1"/>
       <c r="G82" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C83" t="s">
+        <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="E83" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G83" t="s">
         <v>18</v>
@@ -3120,174 +3219,177 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C84" t="s">
+        <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="E84" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F84" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="G84" t="s">
-        <v>18</v>
-      </c>
-      <c r="H84" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>47</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="B85" t="s">
+        <v>38</v>
       </c>
       <c r="C85" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E85" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>47</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="B86" t="s">
+        <v>38</v>
       </c>
       <c r="C86" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D86" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E86" t="s">
-        <v>18</v>
-      </c>
-      <c r="F86" t="s">
+        <v>5</v>
+      </c>
+      <c r="G86" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>48</v>
-      </c>
-      <c r="B87" t="s">
-        <v>34</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" t="s">
+        <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E87" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F87" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G87" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>48</v>
-      </c>
-      <c r="B88" t="s">
-        <v>34</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>38</v>
       </c>
       <c r="D88" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E88" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F88" t="s">
-        <v>18</v>
-      </c>
-      <c r="G88" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C89" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" t="s">
         <v>38</v>
       </c>
-      <c r="D89" t="s">
-        <v>6</v>
-      </c>
       <c r="E89" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F89" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C90" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" t="s">
         <v>38</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>25</v>
       </c>
-      <c r="E90" t="s">
-        <v>18</v>
-      </c>
       <c r="F90" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" t="s">
         <v>22</v>
       </c>
       <c r="D91" t="s">
+        <v>34</v>
+      </c>
+      <c r="E91" t="s">
         <v>38</v>
       </c>
-      <c r="E91" t="s">
-        <v>6</v>
-      </c>
       <c r="F91" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
@@ -3295,633 +3397,624 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" t="s">
         <v>22</v>
       </c>
       <c r="D92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" t="s">
         <v>38</v>
       </c>
-      <c r="E92" t="s">
-        <v>25</v>
-      </c>
       <c r="F92" t="s">
-        <v>18</v>
-      </c>
-      <c r="G92" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>33</v>
+        <v>33</v>
+      </c>
+      <c r="C93" t="s">
+        <v>74</v>
       </c>
       <c r="D93" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E93" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="F93" t="s">
-        <v>6</v>
-      </c>
-      <c r="G93" t="s">
-        <v>18</v>
-      </c>
-      <c r="H93" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>33</v>
+        <v>33</v>
+      </c>
+      <c r="C94" t="s">
+        <v>74</v>
       </c>
       <c r="D94" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E94" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F94" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G94" t="s">
-        <v>18</v>
-      </c>
-      <c r="H94" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>74</v>
+      </c>
+      <c r="E95" t="s">
         <v>38</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E95" s="1"/>
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" t="s">
+        <v>74</v>
+      </c>
+      <c r="E96" t="s">
+        <v>38</v>
+      </c>
+      <c r="F96" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" t="s">
+        <v>18</v>
+      </c>
+      <c r="H96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>47</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C97" t="s">
+        <v>38</v>
+      </c>
+      <c r="D97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" t="s">
+        <v>18</v>
+      </c>
+      <c r="F97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G97" t="s">
+        <v>18</v>
+      </c>
+      <c r="H97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>47</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C98" t="s">
+        <v>38</v>
+      </c>
+      <c r="D98" t="s">
+        <v>25</v>
+      </c>
+      <c r="E98" t="s">
+        <v>18</v>
+      </c>
+      <c r="F98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>48</v>
+      </c>
+      <c r="B99" t="s">
+        <v>34</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D99" t="s">
+        <v>38</v>
+      </c>
+      <c r="E99" t="s">
+        <v>6</v>
+      </c>
+      <c r="F99" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>48</v>
+      </c>
+      <c r="B100" t="s">
+        <v>34</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D100" t="s">
+        <v>38</v>
+      </c>
+      <c r="E100" t="s">
+        <v>25</v>
+      </c>
+      <c r="F100" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>48</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C101" t="s">
+        <v>38</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" t="s">
+        <v>18</v>
+      </c>
+      <c r="F101" t="s">
+        <v>5</v>
+      </c>
+      <c r="G101" s="1"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>48</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C102" t="s">
+        <v>38</v>
+      </c>
+      <c r="D102" t="s">
+        <v>25</v>
+      </c>
+      <c r="E102" t="s">
+        <v>18</v>
+      </c>
+      <c r="F102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>49</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D103" t="s">
+        <v>38</v>
+      </c>
+      <c r="E103" t="s">
+        <v>6</v>
+      </c>
+      <c r="F103" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>49</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" t="s">
+        <v>38</v>
+      </c>
+      <c r="E104" t="s">
+        <v>25</v>
+      </c>
+      <c r="F104" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>50</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D105" t="s">
+        <v>22</v>
+      </c>
+      <c r="E105" t="s">
+        <v>38</v>
+      </c>
+      <c r="F105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>50</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" t="s">
+        <v>38</v>
+      </c>
+      <c r="F106" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>42</v>
+      </c>
+      <c r="B107" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E107" s="1"/>
+      <c r="G107" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>39</v>
       </c>
-      <c r="B96" t="s">
-        <v>75</v>
-      </c>
-      <c r="C96" s="1" t="s">
+      <c r="B108" t="s">
+        <v>73</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D108" t="s">
         <v>19</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E108" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>40</v>
       </c>
-      <c r="B97" t="s">
-        <v>11</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D109" t="s">
         <v>19</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E109" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>51</v>
       </c>
-      <c r="B98" t="s">
-        <v>11</v>
-      </c>
-      <c r="C98" t="s">
-        <v>75</v>
-      </c>
-      <c r="D98" s="1" t="s">
+      <c r="B110" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" t="s">
+        <v>74</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E110" t="s">
         <v>19</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F110" t="s">
         <v>20</v>
       </c>
-      <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>41</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D111" t="s">
         <v>19</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E111" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="G111" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>43</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="B112" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D112" t="s">
         <v>19</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E112" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>44</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C101" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" s="1" t="s">
+      <c r="B113" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C113" t="s">
+        <v>22</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E113" t="s">
         <v>19</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F113" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>45</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D102" s="1" t="s">
+      <c r="B114" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E114" t="s">
         <v>19</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F114" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>52</v>
       </c>
-      <c r="B103" t="s">
-        <v>11</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D103" s="1" t="s">
+      <c r="B115" t="s">
+        <v>11</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E115" t="s">
         <v>19</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F115" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>46</v>
       </c>
-      <c r="B104" t="s">
-        <v>11</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D104" t="s">
-        <v>75</v>
-      </c>
-      <c r="E104" s="1" t="s">
+      <c r="B116" t="s">
+        <v>11</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D116" t="s">
+        <v>74</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F116" t="s">
         <v>19</v>
       </c>
-      <c r="G104" t="s">
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>47</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E117" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>47</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C105" s="1" t="s">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>48</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E118" t="s">
         <v>19</v>
       </c>
-      <c r="E105" t="s">
+      <c r="F118" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>48</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D106" s="1" t="s">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>49</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E119" t="s">
         <v>19</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F119" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>49</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D107" s="1" t="s">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>50</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D120" t="s">
+        <v>22</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F120" t="s">
         <v>19</v>
       </c>
-      <c r="F107" t="s">
+      <c r="G120" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>50</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D108" t="s">
-        <v>22</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F108" t="s">
-        <v>19</v>
-      </c>
-      <c r="G108" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>26</v>
       </c>
-      <c r="B109" t="s">
-        <v>75</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="B121" t="s">
         <v>74</v>
       </c>
-      <c r="E109" t="s">
+      <c r="C121" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D121" t="s">
+        <v>72</v>
+      </c>
+      <c r="E121" t="s">
         <v>35</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F121" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>27</v>
       </c>
-      <c r="B110" t="s">
-        <v>11</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D110" t="s">
-        <v>74</v>
-      </c>
-      <c r="E110" t="s">
-        <v>35</v>
-      </c>
-      <c r="F110" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>28</v>
-      </c>
-      <c r="B111" t="s">
-        <v>11</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E111" t="s">
-        <v>74</v>
-      </c>
-      <c r="F111" t="s">
-        <v>35</v>
-      </c>
-      <c r="G111" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>29</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C112" t="s">
-        <v>74</v>
-      </c>
-      <c r="D112" t="s">
-        <v>35</v>
-      </c>
-      <c r="E112" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>45</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D113" t="s">
-        <v>74</v>
-      </c>
-      <c r="E113" t="s">
-        <v>35</v>
-      </c>
-      <c r="F113" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>52</v>
-      </c>
-      <c r="B114" t="s">
-        <v>11</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D114" t="s">
-        <v>74</v>
-      </c>
-      <c r="E114" t="s">
-        <v>35</v>
-      </c>
-      <c r="F114" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>46</v>
-      </c>
-      <c r="B115" t="s">
-        <v>11</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E115" t="s">
-        <v>74</v>
-      </c>
-      <c r="F115" t="s">
-        <v>35</v>
-      </c>
-      <c r="G115" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>47</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C116" t="s">
-        <v>74</v>
-      </c>
-      <c r="D116" t="s">
-        <v>35</v>
-      </c>
-      <c r="E116" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>50</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D117" t="s">
-        <v>22</v>
-      </c>
-      <c r="E117" t="s">
-        <v>74</v>
-      </c>
-      <c r="F117" t="s">
-        <v>35</v>
-      </c>
-      <c r="G117" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>49</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C118" t="s">
-        <v>22</v>
-      </c>
-      <c r="D118" t="s">
-        <v>74</v>
-      </c>
-      <c r="E118" t="s">
-        <v>35</v>
-      </c>
-      <c r="F118" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>57</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E119" t="s">
-        <v>74</v>
-      </c>
-      <c r="F119" t="s">
-        <v>35</v>
-      </c>
-      <c r="G119" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>58</v>
-      </c>
-      <c r="B120" t="s">
-        <v>11</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E120" t="s">
-        <v>74</v>
-      </c>
-      <c r="F120" t="s">
-        <v>35</v>
-      </c>
-      <c r="G120" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>59</v>
-      </c>
-      <c r="B121" t="s">
-        <v>11</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F121" t="s">
-        <v>74</v>
-      </c>
-      <c r="G121" t="s">
-        <v>35</v>
-      </c>
-      <c r="H121" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>60</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>33</v>
+      <c r="B122" t="s">
+        <v>11</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D122" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E122" t="s">
         <v>35</v>
@@ -3929,22 +4022,25 @@
       <c r="F122" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G122" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>61</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="B123" t="s">
+        <v>11</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E123" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F123" t="s">
         <v>35</v>
@@ -3953,67 +4049,55 @@
         <v>56</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>62</v>
-      </c>
-      <c r="B124" t="s">
-        <v>11</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C124" t="s">
+        <v>72</v>
+      </c>
+      <c r="D124" t="s">
+        <v>35</v>
       </c>
       <c r="E124" t="s">
-        <v>74</v>
-      </c>
-      <c r="F124" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>45</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D125" t="s">
+        <v>72</v>
+      </c>
+      <c r="E125" t="s">
         <v>35</v>
       </c>
-      <c r="G124" t="s">
+      <c r="F125" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>63</v>
-      </c>
-      <c r="B125" t="s">
-        <v>11</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F125" t="s">
-        <v>74</v>
-      </c>
-      <c r="G125" t="s">
-        <v>35</v>
-      </c>
-      <c r="H125" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>64</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
+      </c>
+      <c r="B126" t="s">
+        <v>11</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D126" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E126" t="s">
         <v>35</v>
@@ -4021,384 +4105,1300 @@
       <c r="F126" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G126" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>46</v>
+      </c>
+      <c r="B127" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E127" t="s">
+        <v>72</v>
+      </c>
+      <c r="F127" t="s">
+        <v>35</v>
+      </c>
+      <c r="G127" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>47</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C128" t="s">
+        <v>72</v>
+      </c>
+      <c r="D128" t="s">
+        <v>35</v>
+      </c>
+      <c r="E128" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>50</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D129" t="s">
+        <v>22</v>
+      </c>
+      <c r="E129" t="s">
+        <v>72</v>
+      </c>
+      <c r="F129" t="s">
+        <v>35</v>
+      </c>
+      <c r="G129" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>49</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C130" t="s">
+        <v>22</v>
+      </c>
+      <c r="D130" t="s">
+        <v>72</v>
+      </c>
+      <c r="E130" t="s">
+        <v>35</v>
+      </c>
+      <c r="F130" t="s">
+        <v>56</v>
+      </c>
+      <c r="G130" t="s">
+        <v>35</v>
+      </c>
+      <c r="H130" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>57</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E131" t="s">
+        <v>72</v>
+      </c>
+      <c r="F131" t="s">
+        <v>35</v>
+      </c>
+      <c r="G131" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>58</v>
+      </c>
+      <c r="B132" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E132" t="s">
+        <v>72</v>
+      </c>
+      <c r="F132" t="s">
+        <v>35</v>
+      </c>
+      <c r="G132" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>59</v>
+      </c>
+      <c r="B133" t="s">
+        <v>11</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F133" t="s">
+        <v>72</v>
+      </c>
+      <c r="G133" t="s">
+        <v>35</v>
+      </c>
+      <c r="H133" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>60</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D134" t="s">
+        <v>72</v>
+      </c>
+      <c r="E134" t="s">
+        <v>35</v>
+      </c>
+      <c r="F134" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>61</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E135" t="s">
+        <v>72</v>
+      </c>
+      <c r="F135" t="s">
+        <v>35</v>
+      </c>
+      <c r="G135" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>62</v>
+      </c>
+      <c r="B136" t="s">
+        <v>11</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E136" t="s">
+        <v>72</v>
+      </c>
+      <c r="F136" t="s">
+        <v>35</v>
+      </c>
+      <c r="G136" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>63</v>
+      </c>
+      <c r="B137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F137" t="s">
+        <v>72</v>
+      </c>
+      <c r="G137" t="s">
+        <v>35</v>
+      </c>
+      <c r="H137" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>64</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D138" t="s">
+        <v>72</v>
+      </c>
+      <c r="E138" t="s">
+        <v>35</v>
+      </c>
+      <c r="F138" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>65</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D127" s="1" t="s">
+      <c r="B139" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E127" t="s">
-        <v>22</v>
-      </c>
-      <c r="F127" t="s">
+      <c r="E139" t="s">
+        <v>22</v>
+      </c>
+      <c r="F139" t="s">
+        <v>72</v>
+      </c>
+      <c r="G139" t="s">
+        <v>35</v>
+      </c>
+      <c r="H139" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>66</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D140" t="s">
+        <v>22</v>
+      </c>
+      <c r="E140" t="s">
+        <v>72</v>
+      </c>
+      <c r="F140" t="s">
+        <v>35</v>
+      </c>
+      <c r="G140" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>26</v>
+      </c>
+      <c r="B141" t="s">
         <v>74</v>
       </c>
-      <c r="G127" t="s">
+      <c r="C141" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D141" t="s">
+        <v>72</v>
+      </c>
+      <c r="E141" t="s">
         <v>35</v>
       </c>
-      <c r="H127" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="F141" t="s">
+        <v>88</v>
+      </c>
+      <c r="G141" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>27</v>
+      </c>
+      <c r="B142" t="s">
+        <v>11</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D142" t="s">
+        <v>72</v>
+      </c>
+      <c r="E142" t="s">
+        <v>35</v>
+      </c>
+      <c r="F142" t="s">
+        <v>88</v>
+      </c>
+      <c r="G142" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>28</v>
+      </c>
+      <c r="B143" t="s">
+        <v>11</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E143" t="s">
+        <v>72</v>
+      </c>
+      <c r="F143" t="s">
+        <v>35</v>
+      </c>
+      <c r="G143" t="s">
+        <v>88</v>
+      </c>
+      <c r="H143" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>29</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C144" t="s">
+        <v>72</v>
+      </c>
+      <c r="D144" t="s">
+        <v>35</v>
+      </c>
+      <c r="E144" t="s">
+        <v>88</v>
+      </c>
+      <c r="F144" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>45</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D145" t="s">
+        <v>72</v>
+      </c>
+      <c r="E145" t="s">
+        <v>35</v>
+      </c>
+      <c r="F145" t="s">
+        <v>88</v>
+      </c>
+      <c r="G145" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>52</v>
+      </c>
+      <c r="B146" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D146" t="s">
+        <v>72</v>
+      </c>
+      <c r="E146" t="s">
+        <v>35</v>
+      </c>
+      <c r="F146" t="s">
+        <v>88</v>
+      </c>
+      <c r="G146" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>46</v>
+      </c>
+      <c r="B147" t="s">
+        <v>11</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E147" t="s">
+        <v>72</v>
+      </c>
+      <c r="F147" t="s">
+        <v>35</v>
+      </c>
+      <c r="G147" t="s">
+        <v>88</v>
+      </c>
+      <c r="H147" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>47</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C148" t="s">
+        <v>72</v>
+      </c>
+      <c r="D148" t="s">
+        <v>35</v>
+      </c>
+      <c r="E148" t="s">
+        <v>88</v>
+      </c>
+      <c r="F148" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>50</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D149" t="s">
+        <v>22</v>
+      </c>
+      <c r="E149" t="s">
+        <v>72</v>
+      </c>
+      <c r="F149" t="s">
+        <v>35</v>
+      </c>
+      <c r="G149" t="s">
+        <v>88</v>
+      </c>
+      <c r="H149" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>49</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C150" t="s">
+        <v>22</v>
+      </c>
+      <c r="D150" t="s">
+        <v>72</v>
+      </c>
+      <c r="E150" t="s">
+        <v>35</v>
+      </c>
+      <c r="F150" t="s">
+        <v>88</v>
+      </c>
+      <c r="G150" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>57</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E151" t="s">
+        <v>72</v>
+      </c>
+      <c r="F151" t="s">
+        <v>35</v>
+      </c>
+      <c r="G151" t="s">
+        <v>88</v>
+      </c>
+      <c r="H151" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>58</v>
+      </c>
+      <c r="B152" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E152" t="s">
+        <v>72</v>
+      </c>
+      <c r="F152" t="s">
+        <v>35</v>
+      </c>
+      <c r="G152" t="s">
+        <v>88</v>
+      </c>
+      <c r="H152" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>59</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F153" t="s">
+        <v>72</v>
+      </c>
+      <c r="G153" t="s">
+        <v>35</v>
+      </c>
+      <c r="H153" t="s">
+        <v>88</v>
+      </c>
+      <c r="I153" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>60</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D154" t="s">
+        <v>72</v>
+      </c>
+      <c r="E154" t="s">
+        <v>35</v>
+      </c>
+      <c r="F154" t="s">
+        <v>88</v>
+      </c>
+      <c r="G154" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>61</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E155" t="s">
+        <v>72</v>
+      </c>
+      <c r="F155" t="s">
+        <v>35</v>
+      </c>
+      <c r="G155" t="s">
+        <v>88</v>
+      </c>
+      <c r="H155" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>62</v>
+      </c>
+      <c r="B156" t="s">
+        <v>11</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E156" t="s">
+        <v>72</v>
+      </c>
+      <c r="F156" t="s">
+        <v>35</v>
+      </c>
+      <c r="G156" t="s">
+        <v>88</v>
+      </c>
+      <c r="H156" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>63</v>
+      </c>
+      <c r="B157" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F157" t="s">
+        <v>72</v>
+      </c>
+      <c r="G157" t="s">
+        <v>35</v>
+      </c>
+      <c r="H157" t="s">
+        <v>88</v>
+      </c>
+      <c r="I157" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>64</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D158" t="s">
+        <v>72</v>
+      </c>
+      <c r="E158" t="s">
+        <v>35</v>
+      </c>
+      <c r="F158" t="s">
+        <v>88</v>
+      </c>
+      <c r="G158" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>65</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E159" t="s">
+        <v>22</v>
+      </c>
+      <c r="F159" t="s">
+        <v>72</v>
+      </c>
+      <c r="G159" t="s">
+        <v>35</v>
+      </c>
+      <c r="H159" t="s">
+        <v>88</v>
+      </c>
+      <c r="I159" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>66</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C128" s="1" t="s">
+      <c r="B160" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D128" t="s">
-        <v>22</v>
-      </c>
-      <c r="E128" t="s">
+      <c r="D160" t="s">
+        <v>22</v>
+      </c>
+      <c r="E160" t="s">
+        <v>72</v>
+      </c>
+      <c r="F160" t="s">
+        <v>35</v>
+      </c>
+      <c r="G160" t="s">
+        <v>88</v>
+      </c>
+      <c r="H160" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>81</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>82</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>65</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E164" t="s">
+        <v>25</v>
+      </c>
+      <c r="F164" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>65</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E165" t="s">
+        <v>6</v>
+      </c>
+      <c r="F165" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>83</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D166" s="1"/>
+      <c r="G166" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>17</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>41</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F128" t="s">
-        <v>35</v>
-      </c>
-      <c r="G128" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>49</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>50</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>66</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>65</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D132" t="s">
-        <v>25</v>
-      </c>
-      <c r="E132" t="s">
-        <v>18</v>
-      </c>
-      <c r="F132" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>65</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E133" t="s">
-        <v>6</v>
-      </c>
-      <c r="F133" t="s">
-        <v>18</v>
-      </c>
-      <c r="G133" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>42</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D134" s="1"/>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B135" s="1"/>
-      <c r="C135" s="1"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B136" s="1"/>
-      <c r="C136" s="1"/>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C137" s="1"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D138" s="1"/>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C139" s="1"/>
-      <c r="D139" s="1"/>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B140" s="1"/>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B141" s="1"/>
-      <c r="C141" s="1"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B142" s="1"/>
-      <c r="D142" s="1"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B143" s="1"/>
-      <c r="C143" s="1"/>
-      <c r="D143" s="1"/>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C144" s="1"/>
-      <c r="D144" s="1"/>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C145" s="1"/>
-      <c r="E145" s="1"/>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C146" s="1"/>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
-    </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
-    </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C151" s="1"/>
-    </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D152" s="1"/>
-    </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
-    </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B154" s="1"/>
-    </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
-    </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B156" s="1"/>
-      <c r="D156" s="1"/>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
-    </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
-    </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C159" s="1"/>
-      <c r="E159" s="1"/>
-    </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C160" s="1"/>
-      <c r="D160" s="1"/>
-      <c r="E160" s="1"/>
-    </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
-    </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C162" s="1"/>
-      <c r="D162" s="1"/>
-    </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B163" s="1"/>
-      <c r="C163" s="1"/>
-    </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B164" s="1"/>
-      <c r="C164" s="1"/>
-    </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C165" s="1"/>
-    </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D166" s="1"/>
-    </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-    </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B168" s="1"/>
-    </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B169" s="1"/>
-      <c r="C169" s="1"/>
-    </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B170" s="1"/>
-      <c r="D170" s="1"/>
-    </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B171" s="1"/>
-      <c r="C171" s="1"/>
-      <c r="D171" s="1"/>
-    </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C172" s="1"/>
-      <c r="D172" s="1"/>
-    </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C173" s="1"/>
-      <c r="E173" s="1"/>
-    </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C174" s="1"/>
-      <c r="D174" s="1"/>
-      <c r="E174" s="1"/>
-    </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B175" s="1"/>
-      <c r="C175" s="1"/>
-    </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C176" s="1"/>
-      <c r="D176" s="1"/>
+      <c r="C169" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="177" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B177" s="1"/>
       <c r="C177" s="1"/>
+      <c r="E177" s="1"/>
     </row>
     <row r="178" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B178" s="1"/>
       <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
     </row>
     <row r="179" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B179" s="1"/>
       <c r="C179" s="1"/>
     </row>
     <row r="180" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C180" s="1"/>
       <c r="D180" s="1"/>
     </row>
     <row r="181" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B181" s="1"/>
       <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
     </row>
     <row r="182" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
     </row>
     <row r="183" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B183" s="1"/>
       <c r="C183" s="1"/>
     </row>
     <row r="184" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B184" s="1"/>
       <c r="D184" s="1"/>
     </row>
     <row r="185" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
     </row>
     <row r="186" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C186" s="1"/>
-      <c r="D186" s="1"/>
+      <c r="B186" s="1"/>
     </row>
     <row r="187" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B187" s="1"/>
       <c r="C187" s="1"/>
-      <c r="E187" s="1"/>
     </row>
     <row r="188" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C188" s="1"/>
+      <c r="B188" s="1"/>
       <c r="D188" s="1"/>
-      <c r="E188" s="1"/>
     </row>
     <row r="189" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
+      <c r="D189" s="1"/>
     </row>
     <row r="190" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
+    </row>
+    <row r="191" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C191" s="1"/>
+      <c r="E191" s="1"/>
+    </row>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C192" s="1"/>
+      <c r="D192" s="1"/>
+      <c r="E192" s="1"/>
+    </row>
+    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+    </row>
+    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C194" s="1"/>
+      <c r="D194" s="1"/>
+    </row>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
+    </row>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
+    </row>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C197" s="1"/>
+    </row>
+    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D198" s="1"/>
+    </row>
+    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C199" s="1"/>
+      <c r="D199" s="1"/>
+    </row>
+    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B200" s="1"/>
+    </row>
+    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+    </row>
+    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B202" s="1"/>
+      <c r="D202" s="1"/>
+    </row>
+    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+      <c r="D203" s="1"/>
+    </row>
+    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+    </row>
+    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C205" s="1"/>
+      <c r="E205" s="1"/>
+    </row>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C206" s="1"/>
+      <c r="D206" s="1"/>
+      <c r="E206" s="1"/>
+    </row>
+    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B207" s="1"/>
+      <c r="C207" s="1"/>
+    </row>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C208" s="1"/>
+      <c r="D208" s="1"/>
+    </row>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B209" s="1"/>
+      <c r="C209" s="1"/>
+    </row>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+    </row>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C211" s="1"/>
+    </row>
+    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D212" s="1"/>
+    </row>
+    <row r="213" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C213" s="1"/>
+      <c r="D213" s="1"/>
+    </row>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B214" s="1"/>
+    </row>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B215" s="1"/>
+      <c r="C215" s="1"/>
+    </row>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B216" s="1"/>
+      <c r="D216" s="1"/>
+    </row>
+    <row r="217" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1"/>
+    </row>
+    <row r="218" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C218" s="1"/>
+      <c r="D218" s="1"/>
+    </row>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C219" s="1"/>
+      <c r="E219" s="1"/>
+    </row>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="1"/>
+    </row>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
+    </row>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C222" s="1"/>
+      <c r="D222" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8237,10 +9237,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FAA623-A1BD-4D43-86F2-BAAF15CFDB2B}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8253,92 +9253,192 @@
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>66</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>65</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>72</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -8351,17 +9451,24 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>33</v>
@@ -8370,7 +9477,7 @@
         <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
         <v>35</v>
@@ -8393,7 +9500,7 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
@@ -8410,7 +9517,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>33</v>
@@ -8419,7 +9526,7 @@
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
@@ -8439,7 +9546,7 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -8452,8 +9559,8 @@
       <c r="A5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
+      <c r="B5" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -8465,7 +9572,7 @@
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>35</v>
@@ -8488,7 +9595,7 @@
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>

</xml_diff>